<commit_message>
DONE: just need save to xls
</commit_message>
<xml_diff>
--- a/Planilla excel H.N S.A.-/FEBRERO 2016.-/ALCOSUR_022016.xlsx
+++ b/Planilla excel H.N S.A.-/FEBRERO 2016.-/ALCOSUR_022016.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="55">
   <si>
     <t xml:space="preserve">Nro. de Deposito</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t xml:space="preserve">TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3024 no se encuentra en documentos</t>
   </si>
 </sst>
 </file>
@@ -409,21 +412,21 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="9.14"/>
   </cols>
   <sheetData>
@@ -459,7 +462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>100001461</v>
       </c>
@@ -587,7 +590,7 @@
         <v>68723800</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>100001479</v>
       </c>
@@ -1208,6 +1211,11 @@
       <c r="J25" s="9" t="n">
         <f aca="false">SUM(J2:J24)</f>
         <v>2229417200</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>